<commit_message>
Finished updates to table 2
</commit_message>
<xml_diff>
--- a/output/siber_stats_table.xlsx
+++ b/output/siber_stats_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicablois/Documents/GitHub/LaBrea_smallmamm_isotopes/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{173FE510-616E-0545-B5FC-19B205390263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0ECFCD5-B43B-4547-83B1-782676C26B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="3800" yWindow="10100" windowWidth="28300" windowHeight="10780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="siber_stats_table" sheetId="1" r:id="rId1"/>
@@ -133,10 +133,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -643,15 +640,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -663,9 +654,8 @@
     <xf numFmtId="2" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1020,11 +1010,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1042,28 +1032,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1077,47 +1067,47 @@
       <c r="C2" s="1">
         <v>42</v>
       </c>
-      <c r="D2" s="2">
-        <v>2.7709289487344599</v>
-      </c>
-      <c r="E2" s="2">
-        <v>2.8402021724528201</v>
-      </c>
-      <c r="F2" s="2">
-        <v>2.0226155358445501</v>
-      </c>
-      <c r="G2" s="2">
-        <v>3.7247082483021599</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0.98750000000000004</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0.81247856200253699</v>
+      <c r="D2" s="5">
+        <v>2.7829088855611102</v>
+      </c>
+      <c r="E2" s="5">
+        <v>2.85248160770014</v>
+      </c>
+      <c r="F2" s="5">
+        <v>2.0155688298500301</v>
+      </c>
+      <c r="G2" s="5">
+        <v>3.7247299855407299</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0.98250000000000004</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0.80806077549286803</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="3">
         <v>27</v>
       </c>
       <c r="D3" s="6">
-        <v>4.6896238506238204</v>
+        <v>4.7104154385561499</v>
       </c>
       <c r="E3" s="6">
-        <v>4.8772088046487703</v>
+        <v>4.8988320560984002</v>
       </c>
       <c r="F3" s="6">
-        <v>3.0251163409563699</v>
+        <v>3.0840138438368498</v>
       </c>
       <c r="G3" s="6">
-        <v>6.8451876434086296</v>
-      </c>
-      <c r="H3" s="7"/>
+        <v>6.8220137036014998</v>
+      </c>
+      <c r="H3" s="6"/>
       <c r="I3" s="6">
-        <v>0.47314016465141401</v>
+        <v>0.47051592575588502</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1130,47 +1120,47 @@
       <c r="C4" s="1">
         <v>40</v>
       </c>
-      <c r="D4" s="2">
-        <v>1.8918974302932501</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.9416842047746501</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1.33588666314853</v>
-      </c>
-      <c r="G4" s="2">
-        <v>2.5882124973330698</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0.97875000000000001</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0.73439514539173201</v>
+      <c r="D4" s="5">
+        <v>1.9092959765366999</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1.95954060749819</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1.3672246309695999</v>
+      </c>
+      <c r="G4" s="5">
+        <v>2.5997985511004602</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0.97824999999999995</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0.73495129108706903</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>24</v>
       </c>
       <c r="D5" s="6">
-        <v>3.1557969848594101</v>
+        <v>3.21963437403444</v>
       </c>
       <c r="E5" s="6">
-        <v>3.29924230235302</v>
+        <v>3.3659813910360099</v>
       </c>
       <c r="F5" s="6">
-        <v>1.99850044267241</v>
+        <v>2.0834212831486201</v>
       </c>
       <c r="G5" s="6">
-        <v>4.57992898847401</v>
-      </c>
-      <c r="H5" s="7"/>
+        <v>4.7669781319710696</v>
+      </c>
+      <c r="H5" s="6"/>
       <c r="I5" s="6">
-        <v>0.43220937512046598</v>
+        <v>0.42785943595938702</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1183,30 +1173,30 @@
       <c r="C6" s="1">
         <v>64</v>
       </c>
-      <c r="D6" s="2">
-        <v>3.0803645827575301</v>
-      </c>
-      <c r="E6" s="2">
-        <v>3.1300478824794302</v>
-      </c>
-      <c r="F6" s="2">
-        <v>2.3710654187137701</v>
-      </c>
-      <c r="G6" s="2">
-        <v>3.90218378887689</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0.99299999999999999</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0.57232444870449795</v>
+      <c r="D6" s="5">
+        <v>3.1293811346673102</v>
+      </c>
+      <c r="E6" s="5">
+        <v>3.1798550239361401</v>
+      </c>
+      <c r="F6" s="5">
+        <v>2.4093022881636501</v>
+      </c>
+      <c r="G6" s="5">
+        <v>3.95788454649094</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.99124999999999996</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0.57429633114927303</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>5</v>
       </c>
       <c r="D7" s="6">
@@ -1216,14 +1206,14 @@
         <v>9.2975798892850694</v>
       </c>
       <c r="F7" s="6">
-        <v>2.55203897177595</v>
+        <v>2.34422685486456</v>
       </c>
       <c r="G7" s="6">
-        <v>19.592633430331801</v>
-      </c>
-      <c r="H7" s="7"/>
+        <v>19.3132212421236</v>
+      </c>
+      <c r="H7" s="6"/>
       <c r="I7" s="6">
-        <v>0.19267410983187799</v>
+        <v>0.19641445360831</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1236,46 +1226,46 @@
       <c r="C8" s="1">
         <v>64</v>
       </c>
-      <c r="D8" s="2">
-        <v>3.0803645827575301</v>
-      </c>
-      <c r="E8" s="2">
-        <v>3.1300478824794302</v>
-      </c>
-      <c r="F8" s="2">
-        <v>2.3710654187137701</v>
-      </c>
-      <c r="G8" s="2">
-        <v>3.90218378887689</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0.96225000000000005</v>
-      </c>
-      <c r="I8" s="2" t="s">
+      <c r="D8" s="5">
+        <v>3.1293811346673102</v>
+      </c>
+      <c r="E8" s="5">
+        <v>3.1798550239361401</v>
+      </c>
+      <c r="F8" s="5">
+        <v>2.4093022881636501</v>
+      </c>
+      <c r="G8" s="5">
+        <v>3.95788454649094</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0.95825000000000005</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="3">
         <v>69</v>
       </c>
       <c r="D9" s="6">
-        <v>4.2076803414647799</v>
+        <v>4.24066348004588</v>
       </c>
       <c r="E9" s="6">
-        <v>4.2704815405911196</v>
+        <v>4.3039569648226896</v>
       </c>
       <c r="F9" s="6">
-        <v>3.26486355160494</v>
+        <v>3.3089007975008502</v>
       </c>
       <c r="G9" s="6">
-        <v>5.2884248781640002</v>
-      </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="6" t="s">
+        <v>5.34136658569318</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="4" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
forgot to save table 2 edits
</commit_message>
<xml_diff>
--- a/output/siber_stats_table.xlsx
+++ b/output/siber_stats_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicablois/Documents/GitHub/LaBrea_smallmamm_isotopes/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0ECFCD5-B43B-4547-83B1-782676C26B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0401B0F0-98D2-9F4F-97D5-A404CDB11C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3800" yWindow="10100" windowWidth="28300" windowHeight="10780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -134,6 +134,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -640,9 +643,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -656,6 +662,8 @@
     </xf>
     <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1014,7 +1022,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="H2" sqref="H2:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1032,28 +1040,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1067,46 +1075,46 @@
       <c r="C2" s="1">
         <v>42</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="6">
         <v>2.7829088855611102</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="6">
         <v>2.85248160770014</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="6">
         <v>2.0155688298500301</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="6">
         <v>3.7247299855407299</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="8">
         <v>0.98250000000000004</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="6">
         <v>0.80806077549286803</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>27</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="7">
         <v>4.7104154385561499</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="7">
         <v>4.8988320560984002</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="7">
         <v>3.0840138438368498</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="7">
         <v>6.8220137036014998</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6">
+      <c r="H3" s="9"/>
+      <c r="I3" s="7">
         <v>0.47051592575588502</v>
       </c>
     </row>
@@ -1120,46 +1128,46 @@
       <c r="C4" s="1">
         <v>40</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="6">
         <v>1.9092959765366999</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="6">
         <v>1.95954060749819</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="6">
         <v>1.3672246309695999</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="6">
         <v>2.5997985511004602</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="8">
         <v>0.97824999999999995</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="6">
         <v>0.73495129108706903</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>24</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="7">
         <v>3.21963437403444</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="7">
         <v>3.3659813910360099</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="7">
         <v>2.0834212831486201</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="7">
         <v>4.7669781319710696</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6">
+      <c r="H5" s="9"/>
+      <c r="I5" s="7">
         <v>0.42785943595938702</v>
       </c>
     </row>
@@ -1173,46 +1181,46 @@
       <c r="C6" s="1">
         <v>64</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="6">
         <v>3.1293811346673102</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>3.1798550239361401</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="6">
         <v>2.4093022881636501</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <v>3.95788454649094</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="8">
         <v>0.99124999999999996</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="6">
         <v>0.57429633114927303</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>5</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="7">
         <v>6.9731849169637998</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="7">
         <v>9.2975798892850694</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="7">
         <v>2.34422685486456</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="7">
         <v>19.3132212421236</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6">
+      <c r="H7" s="9"/>
+      <c r="I7" s="7">
         <v>0.19641445360831</v>
       </c>
     </row>
@@ -1226,46 +1234,46 @@
       <c r="C8" s="1">
         <v>64</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="6">
         <v>3.1293811346673102</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="6">
         <v>3.1798550239361401</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="6">
         <v>2.4093022881636501</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="6">
         <v>3.95788454649094</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="8">
         <v>0.95825000000000005</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="4">
         <v>69</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="7">
         <v>4.24066348004588</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="7">
         <v>4.3039569648226896</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="7">
         <v>3.3089007975008502</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="7">
         <v>5.34136658569318</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="4" t="s">
+      <c r="H9" s="9"/>
+      <c r="I9" s="5" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>